<commit_message>
Updated plot of insitu measurements
</commit_message>
<xml_diff>
--- a/data/insitu_flux/insitu_flux_qpoints.xlsx
+++ b/data/insitu_flux/insitu_flux_qpoints.xlsx
@@ -594,11 +594,11 @@
   </sheetPr>
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L52" activeCellId="0" sqref="L52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.18"/>
@@ -2503,7 +2503,7 @@
         <v>4.788</v>
       </c>
       <c r="L51" s="0" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updated in situ data with column descriptions and units
</commit_message>
<xml_diff>
--- a/data/insitu_flux/insitu_flux_qpoints.xlsx
+++ b/data/insitu_flux/insitu_flux_qpoints.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="readme" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="164">
   <si>
     <t xml:space="preserve">stream</t>
   </si>
@@ -473,6 +474,45 @@
   </si>
   <si>
     <t xml:space="preserve">2023-03-08T16:24:00Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stream network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latitude (degrees)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude (degrees)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measurement start time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measurement end time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean co2 flux in umol/m2/sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of observations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">degrees celcius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meq/L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qpoint id</t>
   </si>
 </sst>
 </file>
@@ -485,7 +525,7 @@
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -506,6 +546,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -550,7 +597,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -575,6 +622,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,11 +645,11 @@
   </sheetPr>
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L52" activeCellId="0" sqref="L52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.18"/>
@@ -2667,4 +2718,132 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>